<commit_message>
-Fix iOS test cases -New screens changing procedure -Object model updated due to new UI optimizations and changes
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8180" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCasesData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="328">
   <si>
     <t>Test case</t>
   </si>
@@ -643,9 +643,6 @@
     <t>Mercedes-Benz</t>
   </si>
   <si>
-    <t>CLK-Class</t>
-  </si>
-  <si>
     <t>testTotalSaleSavesWithActiveKeyboardOnWOSummaryScreen</t>
   </si>
   <si>
@@ -1001,6 +998,12 @@
   </si>
   <si>
     <t>Ontario</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>82.03</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1046,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1210,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="163">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -1290,6 +1297,8 @@
     <cellStyle name="Гиперссылка" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -1370,6 +1379,8 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="162" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1700,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1733,28 +1744,28 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" t="s">
         <v>212</v>
       </c>
-      <c r="G1" t="s">
-        <v>213</v>
-      </c>
       <c r="H1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I1" t="s">
         <v>221</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>222</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L1" t="s">
         <v>223</v>
       </c>
-      <c r="K1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>224</v>
-      </c>
-      <c r="M1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -2053,7 +2064,7 @@
         <v>1234</v>
       </c>
       <c r="G13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2211,7 +2222,7 @@
         <v>2004</v>
       </c>
       <c r="F19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H19" s="1">
         <v>95</v>
@@ -2243,7 +2254,7 @@
         <v>2004</v>
       </c>
       <c r="F20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H20" s="1">
         <v>85</v>
@@ -2275,7 +2286,7 @@
         <v>2007</v>
       </c>
       <c r="F21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H21" s="1">
         <v>125</v>
@@ -2305,7 +2316,7 @@
         <v>2008</v>
       </c>
       <c r="F22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H22" s="1">
         <v>265</v>
@@ -2316,7 +2327,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M22" s="1"/>
     </row>
@@ -2976,7 +2987,7 @@
         <v>765106</v>
       </c>
       <c r="G45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -3029,7 +3040,7 @@
         <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E47">
         <v>1995</v>
@@ -3315,8 +3326,8 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
-      <c r="L57" s="1">
-        <v>82.02</v>
+      <c r="L57" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="M57" s="1">
         <v>140.97</v>
@@ -3377,7 +3388,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M59" s="1">
         <v>214</v>
@@ -3452,7 +3463,7 @@
         <v>2006</v>
       </c>
       <c r="F62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -3553,7 +3564,7 @@
         <v>206</v>
       </c>
       <c r="D66" t="s">
-        <v>207</v>
+        <v>326</v>
       </c>
       <c r="E66">
         <v>2007</v>
@@ -3569,10 +3580,10 @@
     </row>
     <row r="67" spans="1:13" ht="15.75" customHeight="1">
       <c r="A67" t="s">
+        <v>207</v>
+      </c>
+      <c r="B67" t="s">
         <v>208</v>
-      </c>
-      <c r="B67" t="s">
-        <v>209</v>
       </c>
       <c r="C67" t="s">
         <v>74</v>
@@ -3594,10 +3605,10 @@
     </row>
     <row r="68" spans="1:13" ht="15.75" customHeight="1">
       <c r="A68" t="s">
+        <v>209</v>
+      </c>
+      <c r="B68" t="s">
         <v>210</v>
-      </c>
-      <c r="B68" t="s">
-        <v>211</v>
       </c>
       <c r="C68" t="s">
         <v>74</v>
@@ -3635,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3656,40 +3667,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -3697,37 +3708,37 @@
         <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="F2" s="3">
         <v>80211</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H2" s="3">
         <v>56289</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="M2" s="2"/>
     </row>
@@ -3736,25 +3747,25 @@
         <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="F3" s="3">
         <v>60652</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -3767,37 +3778,37 @@
         <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="F4" s="3">
         <v>33018</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="M4" s="2"/>
     </row>
@@ -3806,40 +3817,40 @@
         <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="F5" s="3">
         <v>75218</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3847,28 +3858,28 @@
         <v>90</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -3880,19 +3891,19 @@
         <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
@@ -3907,37 +3918,37 @@
         <v>94</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="M8" s="2"/>
     </row>
@@ -3946,37 +3957,37 @@
         <v>98</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="L9" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M9" s="2"/>
     </row>
@@ -3985,25 +3996,25 @@
         <v>101</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -4016,25 +4027,25 @@
         <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -4047,22 +4058,22 @@
         <v>196</v>
       </c>
       <c r="B12" t="s">
+        <v>322</v>
+      </c>
+      <c r="C12" t="s">
         <v>323</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>324</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>325</v>
-      </c>
-      <c r="E12" t="s">
-        <v>326</v>
       </c>
       <c r="F12">
         <v>14121</v>
       </c>
       <c r="I12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iOS client test cases updates
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="329">
   <si>
     <t>Test case</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>82.03</t>
+  </si>
+  <si>
+    <t>140.98</t>
   </si>
 </sst>
 </file>
@@ -1711,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -3329,8 +3332,8 @@
       <c r="L57" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="M57" s="1">
-        <v>140.97</v>
+      <c r="M57" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
-Changes in DW data
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="1680" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCasesData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="328">
   <si>
     <t>Test case</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>testVINDuplicateCheck</t>
-  </si>
-  <si>
-    <t>3VWKM81K69M491628</t>
   </si>
   <si>
     <t>1FMCU0DG4BK830800</t>
@@ -1049,8 +1046,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1220,7 +1221,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="167">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -1302,6 +1303,8 @@
     <cellStyle name="Гиперссылка" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -1384,6 +1387,8 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="166" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1714,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1747,28 +1752,28 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" t="s">
         <v>211</v>
       </c>
-      <c r="G1" t="s">
-        <v>212</v>
-      </c>
       <c r="H1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" t="s">
         <v>220</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>221</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>224</v>
+      </c>
+      <c r="L1" t="s">
         <v>222</v>
       </c>
-      <c r="K1" t="s">
-        <v>225</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>223</v>
-      </c>
-      <c r="M1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
@@ -1799,7 +1804,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1835,16 +1840,16 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
       <c r="E5">
         <v>2011</v>
@@ -1864,16 +1869,16 @@
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
       </c>
       <c r="E6">
         <v>2001</v>
@@ -1891,16 +1896,16 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
       <c r="E7">
         <v>2011</v>
@@ -1916,16 +1921,16 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
       </c>
       <c r="E8">
         <v>2004</v>
@@ -1941,16 +1946,16 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
       </c>
       <c r="E9">
         <v>2010</v>
@@ -1966,16 +1971,16 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
       </c>
       <c r="E10">
         <v>2011</v>
@@ -1997,16 +2002,16 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
       </c>
       <c r="E11">
         <v>2008</v>
@@ -2022,16 +2027,16 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
       </c>
       <c r="E12">
         <v>2006</v>
@@ -2049,16 +2054,16 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
       </c>
       <c r="E13">
         <v>2005</v>
@@ -2067,7 +2072,7 @@
         <v>1234</v>
       </c>
       <c r="G13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2078,16 +2083,16 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
       </c>
       <c r="E14">
         <v>2006</v>
@@ -2101,16 +2106,16 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
       </c>
       <c r="E15">
         <v>2006</v>
@@ -2124,16 +2129,16 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
       </c>
       <c r="E16">
         <v>2001</v>
@@ -2149,16 +2154,16 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>59</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
       </c>
       <c r="E17">
         <v>1999</v>
@@ -2174,16 +2179,16 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
         <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>63</v>
       </c>
       <c r="E18">
         <v>1991</v>
@@ -2210,22 +2215,22 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s">
-        <v>66</v>
       </c>
       <c r="E19">
         <v>2004</v>
       </c>
       <c r="F19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H19" s="1">
         <v>95</v>
@@ -2242,22 +2247,22 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
         <v>67</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
       </c>
       <c r="E20">
         <v>2004</v>
       </c>
       <c r="F20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H20" s="1">
         <v>85</v>
@@ -2274,22 +2279,22 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" t="s">
-        <v>71</v>
-      </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E21">
         <v>2007</v>
       </c>
       <c r="F21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H21" s="1">
         <v>125</v>
@@ -2304,22 +2309,22 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>73</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>74</v>
-      </c>
-      <c r="D22" t="s">
-        <v>75</v>
       </c>
       <c r="E22">
         <v>2008</v>
       </c>
       <c r="F22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H22" s="1">
         <v>265</v>
@@ -2330,22 +2335,22 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>77</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>79</v>
       </c>
       <c r="E23">
         <v>2005</v>
@@ -2369,16 +2374,16 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
       <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
         <v>80</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>81</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
       </c>
       <c r="E24">
         <v>2011</v>
@@ -2398,16 +2403,16 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
         <v>84</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
         <v>85</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" t="s">
-        <v>86</v>
       </c>
       <c r="E25">
         <v>2002</v>
@@ -2431,16 +2436,16 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
       <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
         <v>87</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
         <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s">
-        <v>89</v>
       </c>
       <c r="E26">
         <v>2004</v>
@@ -2462,16 +2467,16 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
       <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
         <v>90</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
       </c>
       <c r="E27">
         <v>2002</v>
@@ -2487,16 +2492,16 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
         <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s">
-        <v>89</v>
       </c>
       <c r="E28">
         <v>2004</v>
@@ -2510,16 +2515,16 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
       <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
         <v>94</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>95</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>96</v>
-      </c>
-      <c r="D29" t="s">
-        <v>97</v>
       </c>
       <c r="E29">
         <v>2007</v>
@@ -2541,16 +2546,16 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
       <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
         <v>98</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
         <v>99</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" t="s">
-        <v>100</v>
       </c>
       <c r="E30">
         <v>2007</v>
@@ -2572,16 +2577,16 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
       <c r="A31" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
         <v>101</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
         <v>102</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" t="s">
-        <v>103</v>
       </c>
       <c r="E31">
         <v>2001</v>
@@ -2601,16 +2606,16 @@
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
       <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
         <v>104</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>105</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>106</v>
-      </c>
-      <c r="D32" t="s">
-        <v>107</v>
       </c>
       <c r="E32">
         <v>2008</v>
@@ -2630,16 +2635,16 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
       <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
         <v>108</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
         <v>109</v>
-      </c>
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s">
-        <v>110</v>
       </c>
       <c r="E33">
         <v>1989</v>
@@ -2661,16 +2666,16 @@
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
       <c r="A34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" t="s">
         <v>111</v>
       </c>
-      <c r="B34" t="s">
-        <v>112</v>
-      </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34">
         <v>2005</v>
@@ -2694,16 +2699,16 @@
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
       <c r="A35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" t="s">
         <v>113</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
         <v>114</v>
-      </c>
-      <c r="C35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" t="s">
-        <v>115</v>
       </c>
       <c r="E35">
         <v>2009</v>
@@ -2719,16 +2724,16 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
       <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
         <v>117</v>
-      </c>
-      <c r="C36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
       </c>
       <c r="E36">
         <v>2000</v>
@@ -2750,16 +2755,16 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
       <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
         <v>119</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>120</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>121</v>
-      </c>
-      <c r="D37" t="s">
-        <v>122</v>
       </c>
       <c r="E37">
         <v>2011</v>
@@ -2775,16 +2780,16 @@
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
       <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
         <v>123</v>
       </c>
-      <c r="B38" t="s">
-        <v>124</v>
-      </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38">
         <v>1991</v>
@@ -2802,16 +2807,16 @@
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1">
       <c r="A39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" t="s">
         <v>125</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>126</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>127</v>
-      </c>
-      <c r="D39" t="s">
-        <v>128</v>
       </c>
       <c r="E39">
         <v>1996</v>
@@ -2829,16 +2834,16 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1">
       <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
         <v>129</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" t="s">
         <v>130</v>
-      </c>
-      <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" t="s">
-        <v>131</v>
       </c>
       <c r="E40">
         <v>2003</v>
@@ -2860,16 +2865,16 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1">
       <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" t="s">
         <v>132</v>
-      </c>
-      <c r="B41" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" t="s">
-        <v>133</v>
       </c>
       <c r="E41">
         <v>1988</v>
@@ -2891,16 +2896,16 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1">
       <c r="A42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" t="s">
         <v>135</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>136</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>137</v>
-      </c>
-      <c r="D42" t="s">
-        <v>138</v>
       </c>
       <c r="E42">
         <v>1987</v>
@@ -2920,16 +2925,16 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1">
       <c r="A43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" t="s">
         <v>139</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>140</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>141</v>
-      </c>
-      <c r="D43" t="s">
-        <v>142</v>
       </c>
       <c r="E43">
         <v>1991</v>
@@ -2945,16 +2950,16 @@
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1">
       <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
         <v>143</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
         <v>144</v>
-      </c>
-      <c r="C44" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" t="s">
-        <v>145</v>
       </c>
       <c r="E44">
         <v>1987</v>
@@ -2972,16 +2977,16 @@
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1">
       <c r="A45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" t="s">
         <v>146</v>
       </c>
-      <c r="B45" t="s">
-        <v>147</v>
-      </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45">
         <v>2001</v>
@@ -2990,7 +2995,7 @@
         <v>765106</v>
       </c>
       <c r="G45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -3001,16 +3006,16 @@
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
       <c r="A46" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" t="s">
         <v>148</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" t="s">
         <v>149</v>
-      </c>
-      <c r="C46" t="s">
-        <v>127</v>
-      </c>
-      <c r="D46" t="s">
-        <v>150</v>
       </c>
       <c r="E46">
         <v>2006</v>
@@ -3034,16 +3039,16 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
       <c r="A47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" t="s">
         <v>151</v>
       </c>
-      <c r="B47" t="s">
-        <v>152</v>
-      </c>
       <c r="C47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E47">
         <v>1995</v>
@@ -3062,16 +3067,16 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" t="s">
         <v>159</v>
-      </c>
-      <c r="D48" t="s">
-        <v>160</v>
       </c>
       <c r="E48">
         <v>2011</v>
@@ -3089,16 +3094,16 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E49">
         <v>2008</v>
@@ -3116,16 +3121,16 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" t="s">
         <v>18</v>
-      </c>
-      <c r="D50" t="s">
-        <v>19</v>
       </c>
       <c r="E50">
         <v>2008</v>
@@ -3143,16 +3148,16 @@
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1">
       <c r="A51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B51" t="s">
         <v>162</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
         <v>163</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>164</v>
       </c>
       <c r="E51">
         <v>2011</v>
@@ -3168,16 +3173,16 @@
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E52">
         <v>2004</v>
@@ -3193,16 +3198,16 @@
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" t="s">
         <v>168</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>169</v>
-      </c>
-      <c r="D53" t="s">
-        <v>170</v>
       </c>
       <c r="E53">
         <v>2003</v>
@@ -3216,16 +3221,16 @@
     </row>
     <row r="54" spans="1:13" ht="15.75" customHeight="1">
       <c r="A54" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" t="s">
         <v>171</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>172</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>173</v>
-      </c>
-      <c r="D54" t="s">
-        <v>174</v>
       </c>
       <c r="E54">
         <v>1989</v>
@@ -3249,16 +3254,16 @@
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1">
       <c r="A55" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" t="s">
         <v>175</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" t="s">
         <v>176</v>
-      </c>
-      <c r="C55" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" t="s">
-        <v>177</v>
       </c>
       <c r="E55">
         <v>1995</v>
@@ -3278,16 +3283,16 @@
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1">
       <c r="A56" t="s">
+        <v>177</v>
+      </c>
+      <c r="B56" t="s">
         <v>178</v>
       </c>
-      <c r="B56" t="s">
-        <v>179</v>
-      </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E56">
         <v>2003</v>
@@ -3305,16 +3310,16 @@
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1">
       <c r="A57" t="s">
+        <v>179</v>
+      </c>
+      <c r="B57" t="s">
         <v>180</v>
       </c>
-      <c r="B57" t="s">
-        <v>181</v>
-      </c>
       <c r="C57" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" t="s">
         <v>59</v>
-      </c>
-      <c r="D57" t="s">
-        <v>60</v>
       </c>
       <c r="E57">
         <v>2001</v>
@@ -3330,24 +3335,24 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="M57" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" customHeight="1">
       <c r="A58" t="s">
+        <v>182</v>
+      </c>
+      <c r="B58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" t="s">
         <v>183</v>
-      </c>
-      <c r="B58" t="s">
-        <v>182</v>
-      </c>
-      <c r="C58" t="s">
-        <v>26</v>
-      </c>
-      <c r="D58" t="s">
-        <v>184</v>
       </c>
       <c r="E58">
         <v>1992</v>
@@ -3367,16 +3372,16 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" customHeight="1">
       <c r="A59" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" t="s">
         <v>185</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
         <v>186</v>
-      </c>
-      <c r="C59" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" t="s">
-        <v>187</v>
       </c>
       <c r="E59">
         <v>2004</v>
@@ -3391,7 +3396,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M59" s="1">
         <v>214</v>
@@ -3399,16 +3404,16 @@
     </row>
     <row r="60" spans="1:13" ht="15.75" customHeight="1">
       <c r="A60" t="s">
+        <v>187</v>
+      </c>
+      <c r="B60" t="s">
         <v>188</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>189</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>190</v>
-      </c>
-      <c r="D60" t="s">
-        <v>191</v>
       </c>
       <c r="E60">
         <v>1998</v>
@@ -3428,16 +3433,16 @@
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1">
       <c r="A61" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
         <v>44</v>
-      </c>
-      <c r="C61" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" t="s">
-        <v>45</v>
       </c>
       <c r="E61">
         <v>2005</v>
@@ -3451,22 +3456,22 @@
     </row>
     <row r="62" spans="1:13" ht="15.75" customHeight="1">
       <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" t="s">
         <v>193</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
         <v>194</v>
-      </c>
-      <c r="C62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" t="s">
-        <v>195</v>
       </c>
       <c r="E62">
         <v>2006</v>
       </c>
       <c r="F62" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -3479,13 +3484,13 @@
     </row>
     <row r="63" spans="1:13" ht="15.75" customHeight="1">
       <c r="A63" t="s">
+        <v>195</v>
+      </c>
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" t="s">
         <v>196</v>
-      </c>
-      <c r="B63" t="s">
-        <v>198</v>
-      </c>
-      <c r="C63" t="s">
-        <v>197</v>
       </c>
       <c r="D63" s="1">
         <v>100</v>
@@ -3504,16 +3509,16 @@
     </row>
     <row r="64" spans="1:13" ht="15.75" customHeight="1">
       <c r="A64" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" t="s">
         <v>199</v>
       </c>
-      <c r="B64" t="s">
-        <v>200</v>
-      </c>
       <c r="C64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E64">
         <v>2000</v>
@@ -3529,16 +3534,16 @@
     </row>
     <row r="65" spans="1:13" ht="15.75" customHeight="1">
       <c r="A65" t="s">
+        <v>200</v>
+      </c>
+      <c r="B65" t="s">
         <v>201</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" t="s">
         <v>202</v>
-      </c>
-      <c r="C65" t="s">
-        <v>74</v>
-      </c>
-      <c r="D65" t="s">
-        <v>203</v>
       </c>
       <c r="E65">
         <v>2011</v>
@@ -3558,16 +3563,16 @@
     </row>
     <row r="66" spans="1:13" ht="15.75" customHeight="1">
       <c r="A66" t="s">
+        <v>203</v>
+      </c>
+      <c r="B66" t="s">
         <v>204</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>205</v>
       </c>
-      <c r="C66" t="s">
-        <v>206</v>
-      </c>
       <c r="D66" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E66">
         <v>2007</v>
@@ -3583,16 +3588,16 @@
     </row>
     <row r="67" spans="1:13" ht="15.75" customHeight="1">
       <c r="A67" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" t="s">
         <v>207</v>
       </c>
-      <c r="B67" t="s">
-        <v>208</v>
-      </c>
       <c r="C67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D67" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E67">
         <v>2002</v>
@@ -3608,16 +3613,16 @@
     </row>
     <row r="68" spans="1:13" ht="15.75" customHeight="1">
       <c r="A68" t="s">
+        <v>208</v>
+      </c>
+      <c r="B68" t="s">
         <v>209</v>
       </c>
-      <c r="B68" t="s">
-        <v>210</v>
-      </c>
       <c r="C68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E68">
         <v>2010</v>
@@ -3670,105 +3675,105 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="F2" s="3">
         <v>80211</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H2" s="3">
         <v>56289</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>252</v>
       </c>
       <c r="F3" s="3">
         <v>60652</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -3778,111 +3783,111 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="F4" s="3">
         <v>33018</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="F5" s="3">
         <v>75218</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -3891,22 +3896,22 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
@@ -3918,106 +3923,106 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="L9" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>312</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>313</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -4027,28 +4032,28 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>320</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -4058,25 +4063,25 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" t="s">
         <v>322</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>323</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>324</v>
-      </c>
-      <c r="E12" t="s">
-        <v>325</v>
       </c>
       <c r="F12">
         <v>14121</v>
       </c>
       <c r="I12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Update test data for Reconpro iOS project
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -1000,10 +1000,10 @@
     <t>CLK</t>
   </si>
   <si>
-    <t>82.03</t>
-  </si>
-  <si>
-    <t>140.98</t>
+    <t>82.02</t>
+  </si>
+  <si>
+    <t>140.97</t>
   </si>
 </sst>
 </file>
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="M58" sqref="M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
-DW update test data
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="329">
   <si>
     <t>Test case</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>140.97</t>
+  </si>
+  <si>
+    <t>933</t>
   </si>
 </sst>
 </file>
@@ -1719,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1996,8 +1999,8 @@
       <c r="L10" s="1">
         <v>750</v>
       </c>
-      <c r="M10" s="1">
-        <v>930</v>
+      <c r="M10" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
-ReconPro test data update
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -1049,8 +1049,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1224,7 +1226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="169">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -1308,6 +1310,7 @@
     <cellStyle name="Гиперссылка" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -1392,6 +1395,7 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="168" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1723,7 +1727,7 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
-R360: Updated data for DW TCs
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="334">
   <si>
     <t>Test case</t>
   </si>
@@ -1006,7 +1006,22 @@
     <t>140.97</t>
   </si>
   <si>
-    <t>933</t>
+    <t>616</t>
+  </si>
+  <si>
+    <t>936</t>
+  </si>
+  <si>
+    <t>532</t>
+  </si>
+  <si>
+    <t>590</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>480</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1869,8 +1884,8 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1">
-        <v>613</v>
+      <c r="L5" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="M5" s="1"/>
     </row>
@@ -2004,7 +2019,7 @@
         <v>750</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
@@ -2666,8 +2681,8 @@
         <v>92</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="L33" s="1">
-        <v>526</v>
+      <c r="L33" s="1" t="s">
+        <v>330</v>
       </c>
       <c r="M33" s="1"/>
     </row>
@@ -2755,8 +2770,8 @@
         <v>125</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="1">
-        <v>578</v>
+      <c r="L36" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="M36" s="1"/>
     </row>
@@ -2865,8 +2880,8 @@
         <v>100</v>
       </c>
       <c r="K40" s="1"/>
-      <c r="L40" s="1">
-        <v>351</v>
+      <c r="L40" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="M40" s="1"/>
     </row>
@@ -2925,8 +2940,8 @@
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="1">
-        <v>477</v>
+      <c r="L42" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="M42" s="1"/>
     </row>

</xml_diff>

<commit_message>
-Fixes for Reconpro calculations test cases
</commit_message>
<xml_diff>
--- a/TestAutomationProject/data/DentWizardData.xlsx
+++ b/TestAutomationProject/data/DentWizardData.xlsx
@@ -1006,22 +1006,22 @@
     <t>140.97</t>
   </si>
   <si>
-    <t>616</t>
-  </si>
-  <si>
-    <t>936</t>
-  </si>
-  <si>
-    <t>532</t>
-  </si>
-  <si>
-    <t>590</t>
-  </si>
-  <si>
-    <t>360</t>
-  </si>
-  <si>
-    <t>480</t>
+    <t>477</t>
+  </si>
+  <si>
+    <t>351</t>
+  </si>
+  <si>
+    <t>613</t>
+  </si>
+  <si>
+    <t>578</t>
+  </si>
+  <si>
+    <t>933</t>
+  </si>
+  <si>
+    <t>526</t>
   </si>
 </sst>
 </file>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1885,7 +1885,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="M5" s="1"/>
     </row>
@@ -2019,7 +2019,7 @@
         <v>750</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="M33" s="1"/>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="M40" s="1"/>
     </row>
@@ -2941,7 +2941,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="M42" s="1"/>
     </row>

</xml_diff>